<commit_message>
Corrijo datos y graficas
</commit_message>
<xml_diff>
--- a/tablas/bank-paramXGB.xlsx
+++ b/tablas/bank-paramXGB.xlsx
@@ -135,40 +135,40 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2176.0</v>
+        <v>1695.0</v>
       </c>
       <c r="C2" t="n">
-        <v>1419.0</v>
+        <v>936.0</v>
       </c>
       <c r="D2" t="n">
-        <v>35129.0</v>
+        <v>35612.0</v>
       </c>
       <c r="E2" t="n">
-        <v>2464.0</v>
+        <v>2945.0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.6052851182197496</v>
+        <v>0.6442417331812998</v>
       </c>
       <c r="G2" t="n">
-        <v>0.4689655172413793</v>
+        <v>0.36530172413793105</v>
       </c>
       <c r="H2" t="n">
-        <v>0.9611743460654482</v>
+        <v>0.974389843493488</v>
       </c>
       <c r="I2" t="n">
-        <v>0.5284760170006071</v>
+        <v>0.46623573098610926</v>
       </c>
       <c r="J2" t="n">
-        <v>0.9057249684374089</v>
+        <v>0.9057735262697874</v>
       </c>
       <c r="K2" t="n">
-        <v>0.47703819985496065</v>
+        <v>0.41885657686789696</v>
       </c>
       <c r="L2" t="n">
-        <v>0.6713848556243486</v>
+        <v>0.5966123446683449</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8784057214083225</v>
+        <v>0.923807018781053</v>
       </c>
     </row>
     <row r="3">
@@ -178,40 +178,40 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2170.0</v>
+        <v>1702.0</v>
       </c>
       <c r="C3" t="n">
-        <v>1416.0</v>
+        <v>939.0</v>
       </c>
       <c r="D3" t="n">
-        <v>35132.0</v>
+        <v>35609.0</v>
       </c>
       <c r="E3" t="n">
-        <v>2470.0</v>
+        <v>2938.0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6051310652537646</v>
+        <v>0.6444528587656191</v>
       </c>
       <c r="G3" t="n">
-        <v>0.4676724137931034</v>
+        <v>0.36681034482758623</v>
       </c>
       <c r="H3" t="n">
-        <v>0.9612564299004049</v>
+        <v>0.9743077596585312</v>
       </c>
       <c r="I3" t="n">
-        <v>0.5275954291271577</v>
+        <v>0.4675181980497184</v>
       </c>
       <c r="J3" t="n">
-        <v>0.9056521316888414</v>
+        <v>0.905870641934544</v>
       </c>
       <c r="K3" t="n">
-        <v>0.4761422484370402</v>
+        <v>0.42012820708539766</v>
       </c>
       <c r="L3" t="n">
-        <v>0.6704872219853735</v>
+        <v>0.5978178362081035</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8784160850820385</v>
+        <v>0.9238504430167439</v>
       </c>
     </row>
     <row r="4">
@@ -221,40 +221,40 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2171.0</v>
+        <v>1712.0</v>
       </c>
       <c r="C4" t="n">
-        <v>1417.0</v>
+        <v>932.0</v>
       </c>
       <c r="D4" t="n">
-        <v>35131.0</v>
+        <v>35616.0</v>
       </c>
       <c r="E4" t="n">
-        <v>2469.0</v>
+        <v>2928.0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.605072463768116</v>
+        <v>0.6475037821482602</v>
       </c>
       <c r="G4" t="n">
-        <v>0.4678879310344828</v>
+        <v>0.3689655172413793</v>
       </c>
       <c r="H4" t="n">
-        <v>0.961229068622086</v>
+        <v>0.9744992886067637</v>
       </c>
       <c r="I4" t="n">
-        <v>0.5277102576567818</v>
+        <v>0.4700713893465129</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9056521316888414</v>
+        <v>0.9062833835097601</v>
       </c>
       <c r="K4" t="n">
-        <v>0.47625164209069487</v>
+        <v>0.422871461331635</v>
       </c>
       <c r="L4" t="n">
-        <v>0.6706321496676033</v>
+        <v>0.5996304145656313</v>
       </c>
       <c r="M4" t="n">
-        <v>0.8785017512395848</v>
+        <v>0.923903558688107</v>
       </c>
     </row>
     <row r="5">
@@ -264,40 +264,40 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2170.0</v>
+        <v>1719.0</v>
       </c>
       <c r="C5" t="n">
-        <v>1413.0</v>
+        <v>929.0</v>
       </c>
       <c r="D5" t="n">
-        <v>35135.0</v>
+        <v>35619.0</v>
       </c>
       <c r="E5" t="n">
-        <v>2470.0</v>
+        <v>2921.0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.6056377337426737</v>
+        <v>0.6491691842900302</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4676724137931034</v>
+        <v>0.3704741379310345</v>
       </c>
       <c r="H5" t="n">
-        <v>0.9613385137353617</v>
+        <v>0.9745813724417205</v>
       </c>
       <c r="I5" t="n">
-        <v>0.5277879119542745</v>
+        <v>0.4717343578485181</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9057249684374089</v>
+        <v>0.9065261726716519</v>
       </c>
       <c r="K5" t="n">
-        <v>0.4763826182540778</v>
+        <v>0.4246331876831825</v>
       </c>
       <c r="L5" t="n">
-        <v>0.6705158485754763</v>
+        <v>0.6008803489872097</v>
       </c>
       <c r="M5" t="n">
-        <v>0.8784859330005634</v>
+        <v>0.9238813777723403</v>
       </c>
     </row>
     <row r="6">
@@ -307,40 +307,40 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2172.0</v>
+        <v>1729.0</v>
       </c>
       <c r="C6" t="n">
-        <v>1414.0</v>
+        <v>926.0</v>
       </c>
       <c r="D6" t="n">
-        <v>35134.0</v>
+        <v>35622.0</v>
       </c>
       <c r="E6" t="n">
-        <v>2468.0</v>
+        <v>2911.0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6056887897378694</v>
+        <v>0.6512241054613936</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4681034482758621</v>
+        <v>0.3726293103448276</v>
       </c>
       <c r="H6" t="n">
-        <v>0.9613111524570428</v>
+        <v>0.9746634562766773</v>
       </c>
       <c r="I6" t="n">
-        <v>0.5280816921954777</v>
+        <v>0.47402330363262507</v>
       </c>
       <c r="J6" t="n">
-        <v>0.9057492473535982</v>
+        <v>0.9068417985821113</v>
       </c>
       <c r="K6" t="n">
-        <v>0.47668147412058454</v>
+        <v>0.4270403235986943</v>
       </c>
       <c r="L6" t="n">
-        <v>0.670815224433066</v>
+        <v>0.6026509533143413</v>
       </c>
       <c r="M6" t="n">
-        <v>0.8784931064908672</v>
+        <v>0.9237469772862761</v>
       </c>
     </row>
   </sheetData>

</xml_diff>